<commit_message>
Fix loading tags from excel
</commit_message>
<xml_diff>
--- a/tests/resources/ExcelLoaderResource-01.xlsx
+++ b/tests/resources/ExcelLoaderResource-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhudec\Develop\GitHub\net_models\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3835C11B-A8DD-4D8A-BA9E-5FD52C116AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00176F5D-B2F3-4F12-A98E-8DF733B34438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6225" windowWidth="16440" windowHeight="28440" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vlan_definitions" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
   <si>
     <t>a_host</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>dest_interface</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>testing</t>
   </si>
 </sst>
 </file>
@@ -550,10 +556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBBAE14-FD98-474A-92AE-567E835A9549}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +576,7 @@
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -604,8 +610,11 @@
       <c r="K1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -630,8 +639,11 @@
       <c r="K2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -659,10 +671,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FA7479-B2EE-435C-B5B0-C0ED390C7F5D}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +694,7 @@
     <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -728,8 +740,11 @@
       <c r="O1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -763,8 +778,11 @@
       <c r="O2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -790,7 +808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -1091,7 +1109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC7C177-BDCD-4419-A32F-156300228421}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Loading hosts from excel
</commit_message>
<xml_diff>
--- a/tests/resources/ExcelLoaderResource-01.xlsx
+++ b/tests/resources/ExcelLoaderResource-01.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhudec\Develop\GitHub\net_models\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00176F5D-B2F3-4F12-A98E-8DF733B34438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DA199C-AE64-4005-9897-DB0AED16A5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vlan_definitions" sheetId="1" r:id="rId1"/>
-    <sheet name="physical_links" sheetId="2" r:id="rId2"/>
-    <sheet name="l3_links" sheetId="3" r:id="rId3"/>
-    <sheet name="l3_ports" sheetId="5" r:id="rId4"/>
-    <sheet name="templates_ospf" sheetId="4" r:id="rId5"/>
-    <sheet name="bgp_routers" sheetId="6" r:id="rId6"/>
-    <sheet name="bgp_peer_groups" sheetId="7" r:id="rId7"/>
-    <sheet name="bgp_neighbors" sheetId="8" r:id="rId8"/>
+    <sheet name="hosts" sheetId="9" r:id="rId2"/>
+    <sheet name="physical_links" sheetId="2" r:id="rId3"/>
+    <sheet name="l3_links" sheetId="3" r:id="rId4"/>
+    <sheet name="l3_ports" sheetId="5" r:id="rId5"/>
+    <sheet name="templates_ospf" sheetId="4" r:id="rId6"/>
+    <sheet name="bgp_routers" sheetId="6" r:id="rId7"/>
+    <sheet name="bgp_peer_groups" sheetId="7" r:id="rId8"/>
+    <sheet name="bgp_neighbors" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
   <si>
     <t>a_host</t>
   </si>
@@ -227,6 +228,18 @@
   </si>
   <si>
     <t>testing</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>mgmt_host</t>
+  </si>
+  <si>
+    <t>ios_xe</t>
+  </si>
+  <si>
+    <t>one,two</t>
   </si>
 </sst>
 </file>
@@ -555,6 +568,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C447181-4234-499F-916C-6C45C0061685}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBBAE14-FD98-474A-92AE-567E835A9549}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -669,11 +738,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FA7479-B2EE-435C-B5B0-C0ED390C7F5D}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -839,7 +908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A0CFB2-5ED7-4FF0-8B7C-3173D8E895C8}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -891,7 +960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA360C7-6997-40CC-95DA-193FDB9163B3}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -969,7 +1038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757AEEE2-118B-47A1-BA52-FB2790A9D8A9}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1022,7 +1091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67945CF7-3B4E-40CB-A73E-8E75F4612E63}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1105,11 +1174,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC7C177-BDCD-4419-A32F-156300228421}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>